<commit_message>
3, 7, 11, çalışıyor
</commit_message>
<xml_diff>
--- a/src/test/java/0_Resource/CucumberTestSonuçlari.xlsx
+++ b/src/test/java/0_Resource/CucumberTestSonuçlari.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="7">
   <si>
     <t>Login with valid username and password</t>
   </si>
@@ -27,6 +27,12 @@
   </si>
   <si>
     <t>Click on menu items</t>
+  </si>
+  <si>
+    <t>Send and Delete Message</t>
+  </si>
+  <si>
+    <t>Finance Functionality</t>
   </si>
 </sst>
 </file>
@@ -71,7 +77,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -221,6 +227,102 @@
         <v>1</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>